<commit_message>
Added generating reports and clearing data for logs
</commit_message>
<xml_diff>
--- a/reports/templates/template.xlsx
+++ b/reports/templates/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ds\Documents\sdforge\sdforge\app\SQLDataForge\reports\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914201FD-E5E0-4DB6-BC2B-575DBAFFA785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7604E1-0728-464C-A7A0-439709697BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{B95166FB-775D-486B-B850-A607DC8EFDE7}"/>
   </bookViews>
@@ -34,12 +34,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>${TABLE}</t>
   </si>
   <si>
-    <t xml:space="preserve">    Отчет "${report-name}" от ${report-date}</t>
+    <t xml:space="preserve">    Отчет "${report-name}"</t>
+  </si>
+  <si>
+    <t>от ${report-date}</t>
+  </si>
+  <si>
+    <t>Тестовый шаблон</t>
   </si>
 </sst>
 </file>
@@ -57,7 +63,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -73,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,18 +91,9 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -105,7 +102,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -124,6 +121,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323851</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>144067</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Рисунок 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C73E3410-856D-45AA-9C9C-F652F6712722}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="1"/>
+          <a:ext cx="1619250" cy="506016"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -423,29 +475,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F7D1E4-3624-4B0E-AF00-E51500211EAC}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" ht="31.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+    <row r="6" spans="1:4" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:XFD1"/>
+    <mergeCell ref="A5:XFD5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fixes for v2.0 release
</commit_message>
<xml_diff>
--- a/reports/templates/template.xlsx
+++ b/reports/templates/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ds\Documents\sdforge\sdforge\app\SQLDataForge\reports\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7604E1-0728-464C-A7A0-439709697BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBD0281-FD2E-4E64-976B-8F72250BF6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{B95166FB-775D-486B-B850-A607DC8EFDE7}"/>
   </bookViews>
@@ -125,7 +125,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
@@ -478,7 +478,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>